<commit_message>
added the reading of the SMD in bottom layer
</commit_message>
<xml_diff>
--- a/components-list.xlsx
+++ b/components-list.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pferronato/Documents/GitHub/MacCCAB/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{761B0433-433A-6A4F-A586-AC48DD8BB199}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5ED61D2F-E23F-0749-B92D-AF40D23DB7AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{E2A3F92D-8677-E441-96D7-ADFE3F01DE27}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="890" uniqueCount="346">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="963" uniqueCount="384">
   <si>
     <t>Code</t>
   </si>
@@ -824,51 +824,33 @@
     <t>STPR8</t>
   </si>
   <si>
+    <t>CP44</t>
+  </si>
+  <si>
     <t>5600uF 10V</t>
   </si>
   <si>
     <t>CP40</t>
   </si>
   <si>
-    <t>cp14</t>
-  </si>
-  <si>
     <t>1000uf 16v</t>
   </si>
   <si>
-    <t>cp56</t>
-  </si>
-  <si>
     <t>3300uf 16v</t>
   </si>
   <si>
-    <t>cp39</t>
-  </si>
-  <si>
     <t>l7905acv</t>
   </si>
   <si>
-    <t>cp47</t>
-  </si>
-  <si>
     <t>1uf 50v</t>
   </si>
   <si>
     <t>100uf 25v</t>
   </si>
   <si>
-    <t>cp44</t>
-  </si>
-  <si>
-    <t>cp42</t>
-  </si>
-  <si>
     <t>470uf 25v</t>
   </si>
   <si>
-    <t>cp43</t>
-  </si>
-  <si>
     <t>1000uf 35v</t>
   </si>
   <si>
@@ -890,9 +872,6 @@
     <t>G1242</t>
   </si>
   <si>
-    <t>cp31</t>
-  </si>
-  <si>
     <t>6800 63-h wima cn 1%</t>
   </si>
   <si>
@@ -1071,13 +1050,148 @@
   </si>
   <si>
     <t>ES1D</t>
+  </si>
+  <si>
+    <t>CP14</t>
+  </si>
+  <si>
+    <t>CP31</t>
+  </si>
+  <si>
+    <t>CP39</t>
+  </si>
+  <si>
+    <t>CP42</t>
+  </si>
+  <si>
+    <t>CP43</t>
+  </si>
+  <si>
+    <t>CP47</t>
+  </si>
+  <si>
+    <t>CP56</t>
+  </si>
+  <si>
+    <t>RP12</t>
+  </si>
+  <si>
+    <t>Thermistor PTH451C</t>
+  </si>
+  <si>
+    <t>PTH451C</t>
+  </si>
+  <si>
+    <t>CP2</t>
+  </si>
+  <si>
+    <t>103Z 2KV</t>
+  </si>
+  <si>
+    <t>0.01uF 2000V</t>
+  </si>
+  <si>
+    <t>CP10</t>
+  </si>
+  <si>
+    <t>1uF 50V</t>
+  </si>
+  <si>
+    <t>1A3</t>
+  </si>
+  <si>
+    <t>0.001uF ??</t>
+  </si>
+  <si>
+    <t>N2</t>
+  </si>
+  <si>
+    <t>IJ5</t>
+  </si>
+  <si>
+    <t>220nF</t>
+  </si>
+  <si>
+    <t>IA3</t>
+  </si>
+  <si>
+    <t>IJ4</t>
+  </si>
+  <si>
+    <t>DP15</t>
+  </si>
+  <si>
+    <t>A6P</t>
+  </si>
+  <si>
+    <t>?</t>
+  </si>
+  <si>
+    <t>0 is uncertain</t>
+  </si>
+  <si>
+    <t>DP18</t>
+  </si>
+  <si>
+    <t>DP uncertain</t>
+  </si>
+  <si>
+    <t>IJ3</t>
+  </si>
+  <si>
+    <t>I?4</t>
+  </si>
+  <si>
+    <t>CL5</t>
+  </si>
+  <si>
+    <t>3A</t>
+  </si>
+  <si>
+    <t>line above, A is maybe a lambda</t>
+  </si>
+  <si>
+    <t>3FP 2N</t>
+  </si>
+  <si>
+    <t>Y12 2N</t>
+  </si>
+  <si>
+    <t>CL3</t>
+  </si>
+  <si>
+    <t>maybe A is a kambda</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CV1 </t>
+  </si>
+  <si>
+    <t>1A4</t>
+  </si>
+  <si>
+    <t>maybe 1 is I</t>
+  </si>
+  <si>
+    <t>E2</t>
+  </si>
+  <si>
+    <t>a line above</t>
+  </si>
+  <si>
+    <t>CV16</t>
+  </si>
+  <si>
+    <t>J4</t>
+  </si>
+  <si>
+    <t>0.33nF line above</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1088,6 +1202,14 @@
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1140,14 +1262,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1177,10 +1300,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{2EA5F103-BD9C-724C-A7B1-1465ACBA67A0}" name="Table1" displayName="Table1" ref="A1:E266" totalsRowShown="0">
-  <autoFilter ref="A1:E266" xr:uid="{2EA5F103-BD9C-724C-A7B1-1465ACBA67A0}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E265">
-    <sortCondition ref="A1:A266"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{2EA5F103-BD9C-724C-A7B1-1465ACBA67A0}" name="Table1" displayName="Table1" ref="A1:E276" totalsRowShown="0">
+  <autoFilter ref="A1:E276" xr:uid="{2EA5F103-BD9C-724C-A7B1-1465ACBA67A0}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E276">
+    <sortCondition ref="A1:A276"/>
   </sortState>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{3B152FFC-0A64-E142-BE73-9D91DF7AE0AD}" name="Code"/>
@@ -1490,10 +1613,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E99BFAA7-9D71-9746-8250-F1CFD200436D}">
-  <dimension ref="A1:E265"/>
+  <dimension ref="A1:E276"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A114" zoomScale="150" workbookViewId="0">
-      <selection activeCell="B118" sqref="B118"/>
+    <sheetView tabSelected="1" zoomScale="99" workbookViewId="0">
+      <selection activeCell="A51" sqref="A51:XFD51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1518,7 +1641,7 @@
         <v>1</v>
       </c>
       <c r="E1" t="s">
-        <v>289</v>
+        <v>282</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
@@ -1569,17 +1692,26 @@
       <c r="A6" t="s">
         <v>201</v>
       </c>
+      <c r="B6" t="s">
+        <v>377</v>
+      </c>
       <c r="C6" t="s">
         <v>108</v>
       </c>
       <c r="D6" t="s">
         <v>4</v>
+      </c>
+      <c r="E6" t="s">
+        <v>378</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>11</v>
       </c>
+      <c r="B7" t="s">
+        <v>367</v>
+      </c>
       <c r="C7" t="s">
         <v>186</v>
       </c>
@@ -1624,6 +1756,9 @@
       <c r="A11" t="s">
         <v>12</v>
       </c>
+      <c r="B11" t="s">
+        <v>357</v>
+      </c>
       <c r="C11" t="s">
         <v>186</v>
       </c>
@@ -1660,17 +1795,26 @@
       <c r="A14" t="s">
         <v>200</v>
       </c>
+      <c r="B14" t="s">
+        <v>379</v>
+      </c>
       <c r="C14" t="s">
         <v>108</v>
       </c>
       <c r="D14" t="s">
         <v>4</v>
+      </c>
+      <c r="E14" t="s">
+        <v>380</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>23</v>
       </c>
+      <c r="B15" t="s">
+        <v>235</v>
+      </c>
       <c r="C15" t="s">
         <v>186</v>
       </c>
@@ -1682,6 +1826,9 @@
       <c r="A16" t="s">
         <v>34</v>
       </c>
+      <c r="B16" t="s">
+        <v>357</v>
+      </c>
       <c r="C16" t="s">
         <v>187</v>
       </c>
@@ -1693,6 +1840,9 @@
       <c r="A17" t="s">
         <v>37</v>
       </c>
+      <c r="B17" t="s">
+        <v>368</v>
+      </c>
       <c r="C17" t="s">
         <v>187</v>
       </c>
@@ -1702,35 +1852,39 @@
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>221</v>
-      </c>
-      <c r="C18" t="s">
-        <v>108</v>
-      </c>
-      <c r="D18" t="s">
-        <v>4</v>
-      </c>
+        <v>374</v>
+      </c>
+      <c r="B18" t="s">
+        <v>357</v>
+      </c>
+      <c r="D18" s="5"/>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>134</v>
+        <v>221</v>
       </c>
       <c r="B19" t="s">
-        <v>45</v>
+        <v>379</v>
       </c>
       <c r="C19" t="s">
         <v>108</v>
       </c>
       <c r="D19" t="s">
         <v>4</v>
+      </c>
+      <c r="E19" t="s">
+        <v>380</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>190</v>
+        <v>134</v>
+      </c>
+      <c r="B20" t="s">
+        <v>45</v>
       </c>
       <c r="C20" t="s">
-        <v>187</v>
+        <v>108</v>
       </c>
       <c r="D20" t="s">
         <v>4</v>
@@ -1738,49 +1892,50 @@
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>85</v>
-      </c>
-      <c r="C21" t="s">
-        <v>148</v>
-      </c>
-      <c r="D21" t="s">
-        <v>4</v>
+        <v>369</v>
+      </c>
+      <c r="B21" t="s">
+        <v>370</v>
+      </c>
+      <c r="D21" s="5"/>
+      <c r="E21" t="s">
+        <v>371</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>265</v>
-      </c>
-      <c r="B22" t="s">
-        <v>266</v>
+        <v>190</v>
       </c>
       <c r="C22" t="s">
-        <v>163</v>
+        <v>187</v>
       </c>
       <c r="D22" t="s">
-        <v>253</v>
+        <v>4</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>158</v>
+        <v>85</v>
       </c>
       <c r="B23" t="s">
-        <v>273</v>
+        <v>357</v>
       </c>
       <c r="C23" t="s">
-        <v>163</v>
+        <v>148</v>
       </c>
       <c r="D23" t="s">
         <v>4</v>
+      </c>
+      <c r="E23" t="s">
+        <v>358</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>319</v>
+        <v>352</v>
       </c>
       <c r="B24" t="s">
-        <v>311</v>
+        <v>353</v>
       </c>
       <c r="C24" t="s">
         <v>148</v>
@@ -1788,27 +1943,30 @@
       <c r="D24" t="s">
         <v>253</v>
       </c>
-      <c r="E24" t="s">
-        <v>312</v>
-      </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>147</v>
+        <v>339</v>
+      </c>
+      <c r="B25" t="s">
+        <v>266</v>
       </c>
       <c r="C25" t="s">
-        <v>148</v>
+        <v>163</v>
       </c>
       <c r="D25" t="s">
-        <v>4</v>
+        <v>253</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>83</v>
+        <v>158</v>
+      </c>
+      <c r="B26" t="s">
+        <v>270</v>
       </c>
       <c r="C26" t="s">
-        <v>148</v>
+        <v>163</v>
       </c>
       <c r="D26" t="s">
         <v>4</v>
@@ -1816,10 +1974,10 @@
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>285</v>
+        <v>312</v>
       </c>
       <c r="B27" t="s">
-        <v>286</v>
+        <v>304</v>
       </c>
       <c r="C27" t="s">
         <v>148</v>
@@ -1827,21 +1985,30 @@
       <c r="D27" t="s">
         <v>253</v>
       </c>
+      <c r="E27" t="s">
+        <v>305</v>
+      </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>149</v>
+        <v>349</v>
+      </c>
+      <c r="B28" t="s">
+        <v>350</v>
       </c>
       <c r="C28" t="s">
         <v>148</v>
       </c>
       <c r="D28" t="s">
-        <v>4</v>
+        <v>253</v>
+      </c>
+      <c r="E28" t="s">
+        <v>351</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>156</v>
+        <v>147</v>
       </c>
       <c r="C29" t="s">
         <v>148</v>
@@ -1852,7 +2019,10 @@
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>153</v>
+        <v>83</v>
+      </c>
+      <c r="B30" t="s">
+        <v>354</v>
       </c>
       <c r="C30" t="s">
         <v>148</v>
@@ -1860,13 +2030,16 @@
       <c r="D30" t="s">
         <v>4</v>
       </c>
+      <c r="E30" t="s">
+        <v>355</v>
+      </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>297</v>
+        <v>340</v>
       </c>
       <c r="B31" t="s">
-        <v>298</v>
+        <v>279</v>
       </c>
       <c r="C31" t="s">
         <v>148</v>
@@ -1877,58 +2050,55 @@
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>269</v>
+        <v>149</v>
       </c>
       <c r="B32" t="s">
-        <v>268</v>
+        <v>360</v>
       </c>
       <c r="C32" t="s">
-        <v>163</v>
+        <v>148</v>
       </c>
       <c r="D32" t="s">
-        <v>253</v>
+        <v>4</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>294</v>
+        <v>156</v>
       </c>
       <c r="B33" t="s">
-        <v>293</v>
+        <v>357</v>
       </c>
       <c r="C33" t="s">
         <v>148</v>
       </c>
       <c r="D33" t="s">
-        <v>253</v>
-      </c>
-      <c r="E33" t="s">
-        <v>296</v>
+        <v>4</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>264</v>
+        <v>153</v>
       </c>
       <c r="B34" t="s">
-        <v>263</v>
+        <v>359</v>
       </c>
       <c r="C34" t="s">
-        <v>163</v>
+        <v>148</v>
       </c>
       <c r="D34" t="s">
-        <v>253</v>
+        <v>4</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>275</v>
+        <v>290</v>
       </c>
       <c r="B35" t="s">
-        <v>263</v>
+        <v>291</v>
       </c>
       <c r="C35" t="s">
-        <v>163</v>
+        <v>148</v>
       </c>
       <c r="D35" t="s">
         <v>253</v>
@@ -1936,10 +2106,10 @@
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>277</v>
+        <v>341</v>
       </c>
       <c r="B36" t="s">
-        <v>278</v>
+        <v>267</v>
       </c>
       <c r="C36" t="s">
         <v>163</v>
@@ -1950,24 +2120,27 @@
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>274</v>
+        <v>287</v>
       </c>
       <c r="B37" t="s">
-        <v>276</v>
+        <v>286</v>
       </c>
       <c r="C37" t="s">
-        <v>163</v>
+        <v>148</v>
       </c>
       <c r="D37" t="s">
         <v>253</v>
       </c>
+      <c r="E37" t="s">
+        <v>289</v>
+      </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>271</v>
+        <v>265</v>
       </c>
       <c r="B38" t="s">
-        <v>272</v>
+        <v>264</v>
       </c>
       <c r="C38" t="s">
         <v>163</v>
@@ -1978,66 +2151,69 @@
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>161</v>
+        <v>342</v>
+      </c>
+      <c r="B39" t="s">
+        <v>264</v>
       </c>
       <c r="C39" t="s">
-        <v>148</v>
+        <v>163</v>
       </c>
       <c r="D39" t="s">
-        <v>4</v>
+        <v>253</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>179</v>
+        <v>343</v>
       </c>
       <c r="B40" t="s">
-        <v>181</v>
+        <v>272</v>
       </c>
       <c r="C40" t="s">
         <v>163</v>
       </c>
       <c r="D40" t="s">
-        <v>4</v>
+        <v>253</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>295</v>
+        <v>263</v>
       </c>
       <c r="B41" t="s">
-        <v>293</v>
+        <v>271</v>
       </c>
       <c r="C41" t="s">
-        <v>148</v>
+        <v>163</v>
       </c>
       <c r="D41" t="s">
         <v>253</v>
       </c>
-      <c r="E41" t="s">
-        <v>296</v>
-      </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>177</v>
+        <v>344</v>
       </c>
       <c r="B42" t="s">
-        <v>181</v>
+        <v>269</v>
       </c>
       <c r="C42" t="s">
         <v>163</v>
       </c>
       <c r="D42" t="s">
-        <v>4</v>
+        <v>253</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>102</v>
+        <v>161</v>
+      </c>
+      <c r="B43" t="s">
+        <v>363</v>
       </c>
       <c r="C43" t="s">
-        <v>163</v>
+        <v>148</v>
       </c>
       <c r="D43" t="s">
         <v>4</v>
@@ -2045,10 +2221,10 @@
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>171</v>
+        <v>179</v>
       </c>
       <c r="B44" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="C44" t="s">
         <v>163</v>
@@ -2059,52 +2235,52 @@
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>72</v>
-      </c>
-      <c r="C45" t="s">
-        <v>148</v>
-      </c>
-      <c r="D45" t="s">
+        <v>179</v>
+      </c>
+      <c r="B45" t="s">
+        <v>235</v>
+      </c>
+      <c r="D45" s="7" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>267</v>
+        <v>288</v>
       </c>
       <c r="B46" t="s">
-        <v>268</v>
+        <v>286</v>
       </c>
       <c r="C46" t="s">
-        <v>163</v>
+        <v>148</v>
       </c>
       <c r="D46" t="s">
         <v>253</v>
       </c>
+      <c r="E46" t="s">
+        <v>289</v>
+      </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>81</v>
+        <v>288</v>
       </c>
       <c r="B47" t="s">
-        <v>45</v>
-      </c>
-      <c r="C47" t="s">
-        <v>148</v>
-      </c>
-      <c r="D47" t="s">
+        <v>357</v>
+      </c>
+      <c r="D47" s="7" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>78</v>
+        <v>177</v>
       </c>
       <c r="B48" t="s">
-        <v>45</v>
+        <v>357</v>
       </c>
       <c r="C48" t="s">
-        <v>148</v>
+        <v>163</v>
       </c>
       <c r="D48" t="s">
         <v>4</v>
@@ -2112,52 +2288,52 @@
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>329</v>
-      </c>
-      <c r="B49" t="s">
-        <v>279</v>
+        <v>102</v>
       </c>
       <c r="C49" t="s">
-        <v>148</v>
+        <v>163</v>
       </c>
       <c r="D49" t="s">
-        <v>253</v>
+        <v>4</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>325</v>
+        <v>171</v>
       </c>
       <c r="B50" t="s">
-        <v>306</v>
+        <v>182</v>
       </c>
       <c r="C50" t="s">
-        <v>148</v>
+        <v>163</v>
       </c>
       <c r="D50" t="s">
-        <v>253</v>
+        <v>4</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>324</v>
+        <v>72</v>
       </c>
       <c r="B51" t="s">
-        <v>338</v>
+        <v>356</v>
       </c>
       <c r="C51" t="s">
         <v>148</v>
       </c>
       <c r="D51" t="s">
-        <v>253</v>
+        <v>4</v>
+      </c>
+      <c r="E51" t="s">
+        <v>383</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>327</v>
+        <v>345</v>
       </c>
       <c r="B52" t="s">
-        <v>281</v>
+        <v>267</v>
       </c>
       <c r="C52" t="s">
         <v>163</v>
@@ -2168,10 +2344,13 @@
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>167</v>
+        <v>81</v>
+      </c>
+      <c r="B53" t="s">
+        <v>45</v>
       </c>
       <c r="C53" t="s">
-        <v>163</v>
+        <v>148</v>
       </c>
       <c r="D53" t="s">
         <v>4</v>
@@ -2179,13 +2358,13 @@
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>94</v>
+        <v>78</v>
       </c>
       <c r="B54" t="s">
         <v>45</v>
       </c>
       <c r="C54" t="s">
-        <v>163</v>
+        <v>148</v>
       </c>
       <c r="D54" t="s">
         <v>4</v>
@@ -2193,60 +2372,69 @@
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>166</v>
+        <v>322</v>
+      </c>
+      <c r="B55" t="s">
+        <v>273</v>
       </c>
       <c r="C55" t="s">
-        <v>163</v>
+        <v>148</v>
       </c>
       <c r="D55" t="s">
-        <v>4</v>
+        <v>253</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>129</v>
+        <v>318</v>
+      </c>
+      <c r="B56" t="s">
+        <v>299</v>
       </c>
       <c r="C56" t="s">
-        <v>108</v>
+        <v>148</v>
       </c>
       <c r="D56" t="s">
-        <v>4</v>
+        <v>253</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>234</v>
+        <v>317</v>
       </c>
       <c r="B57" t="s">
-        <v>235</v>
+        <v>331</v>
       </c>
       <c r="C57" t="s">
-        <v>108</v>
+        <v>148</v>
       </c>
       <c r="D57" t="s">
-        <v>4</v>
-      </c>
-      <c r="E57" t="s">
-        <v>314</v>
+        <v>253</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>247</v>
+        <v>320</v>
+      </c>
+      <c r="B58" t="s">
+        <v>275</v>
       </c>
       <c r="C58" t="s">
-        <v>108</v>
+        <v>163</v>
       </c>
       <c r="D58" t="s">
-        <v>4</v>
+        <v>253</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>251</v>
+        <v>167</v>
+      </c>
+      <c r="B59" t="s">
+        <v>235</v>
       </c>
       <c r="C59" t="s">
-        <v>108</v>
+        <v>163</v>
       </c>
       <c r="D59" t="s">
         <v>4</v>
@@ -2254,10 +2442,13 @@
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>233</v>
+        <v>94</v>
+      </c>
+      <c r="B60" t="s">
+        <v>45</v>
       </c>
       <c r="C60" t="s">
-        <v>108</v>
+        <v>163</v>
       </c>
       <c r="D60" t="s">
         <v>4</v>
@@ -2265,10 +2456,10 @@
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>227</v>
+        <v>166</v>
       </c>
       <c r="C61" t="s">
-        <v>108</v>
+        <v>163</v>
       </c>
       <c r="D61" t="s">
         <v>4</v>
@@ -2276,7 +2467,10 @@
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>130</v>
+        <v>129</v>
+      </c>
+      <c r="B62" t="s">
+        <v>382</v>
       </c>
       <c r="C62" t="s">
         <v>108</v>
@@ -2287,7 +2481,10 @@
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>132</v>
+        <v>376</v>
+      </c>
+      <c r="B63" t="s">
+        <v>235</v>
       </c>
       <c r="C63" t="s">
         <v>108</v>
@@ -2298,7 +2495,7 @@
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="B64" t="s">
         <v>235</v>
@@ -2310,12 +2507,12 @@
         <v>4</v>
       </c>
       <c r="E64" t="s">
-        <v>314</v>
+        <v>307</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>244</v>
+        <v>247</v>
       </c>
       <c r="C65" t="s">
         <v>108</v>
@@ -2326,7 +2523,7 @@
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>133</v>
+        <v>251</v>
       </c>
       <c r="C66" t="s">
         <v>108</v>
@@ -2337,7 +2534,7 @@
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>131</v>
+        <v>233</v>
       </c>
       <c r="C67" t="s">
         <v>108</v>
@@ -2348,7 +2545,7 @@
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>205</v>
+        <v>227</v>
       </c>
       <c r="C68" t="s">
         <v>108</v>
@@ -2359,18 +2556,19 @@
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>231</v>
-      </c>
-      <c r="C69" t="s">
-        <v>108</v>
-      </c>
-      <c r="D69" t="s">
-        <v>4</v>
-      </c>
+        <v>381</v>
+      </c>
+      <c r="B69" t="s">
+        <v>382</v>
+      </c>
+      <c r="D69" s="5"/>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>230</v>
+        <v>130</v>
+      </c>
+      <c r="B70" t="s">
+        <v>235</v>
       </c>
       <c r="C70" t="s">
         <v>108</v>
@@ -2381,7 +2579,7 @@
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>245</v>
+        <v>132</v>
       </c>
       <c r="C71" t="s">
         <v>108</v>
@@ -2392,7 +2590,7 @@
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="B72" t="s">
         <v>235</v>
@@ -2404,12 +2602,12 @@
         <v>4</v>
       </c>
       <c r="E72" t="s">
-        <v>314</v>
+        <v>307</v>
       </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>238</v>
+        <v>244</v>
       </c>
       <c r="B73" t="s">
         <v>235</v>
@@ -2420,27 +2618,27 @@
       <c r="D73" t="s">
         <v>4</v>
       </c>
-      <c r="E73" t="s">
-        <v>314</v>
-      </c>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
-        <v>54</v>
+        <v>133</v>
+      </c>
+      <c r="B74" t="s">
+        <v>235</v>
       </c>
       <c r="C74" t="s">
-        <v>184</v>
+        <v>108</v>
       </c>
       <c r="D74" t="s">
         <v>4</v>
-      </c>
-      <c r="E74" t="s">
-        <v>315</v>
       </c>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
-        <v>111</v>
+        <v>131</v>
+      </c>
+      <c r="B75" t="s">
+        <v>235</v>
       </c>
       <c r="C75" t="s">
         <v>108</v>
@@ -2451,10 +2649,10 @@
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
-        <v>65</v>
+        <v>205</v>
       </c>
       <c r="C76" t="s">
-        <v>187</v>
+        <v>108</v>
       </c>
       <c r="D76" t="s">
         <v>4</v>
@@ -2462,7 +2660,10 @@
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>110</v>
+        <v>231</v>
+      </c>
+      <c r="B77" t="s">
+        <v>235</v>
       </c>
       <c r="C77" t="s">
         <v>108</v>
@@ -2473,10 +2674,13 @@
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
-        <v>10</v>
+        <v>230</v>
+      </c>
+      <c r="B78" t="s">
+        <v>382</v>
       </c>
       <c r="C78" t="s">
-        <v>186</v>
+        <v>108</v>
       </c>
       <c r="D78" t="s">
         <v>4</v>
@@ -2484,126 +2688,114 @@
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
-        <v>287</v>
+        <v>245</v>
       </c>
       <c r="B79" t="s">
-        <v>288</v>
+        <v>235</v>
       </c>
       <c r="C79" t="s">
-        <v>148</v>
+        <v>108</v>
       </c>
       <c r="D79" t="s">
-        <v>253</v>
-      </c>
-      <c r="E79" t="s">
-        <v>290</v>
+        <v>4</v>
       </c>
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
-        <v>154</v>
+        <v>239</v>
       </c>
       <c r="B80" t="s">
-        <v>316</v>
+        <v>235</v>
       </c>
       <c r="C80" t="s">
-        <v>148</v>
+        <v>108</v>
       </c>
       <c r="D80" t="s">
         <v>4</v>
       </c>
       <c r="E80" t="s">
-        <v>317</v>
+        <v>307</v>
       </c>
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
-        <v>261</v>
+        <v>238</v>
       </c>
       <c r="B81" t="s">
-        <v>262</v>
+        <v>235</v>
       </c>
       <c r="C81" t="s">
-        <v>163</v>
+        <v>108</v>
       </c>
       <c r="D81" t="s">
-        <v>253</v>
+        <v>4</v>
+      </c>
+      <c r="E81" t="s">
+        <v>307</v>
       </c>
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
-        <v>76</v>
-      </c>
-      <c r="B82" s="6" t="s">
-        <v>316</v>
-      </c>
-      <c r="C82" s="6" t="s">
-        <v>148</v>
-      </c>
-      <c r="D82" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="C82" t="s">
+        <v>184</v>
+      </c>
+      <c r="D82" t="s">
         <v>4</v>
       </c>
       <c r="E82" t="s">
-        <v>318</v>
+        <v>308</v>
       </c>
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
-        <v>169</v>
+        <v>111</v>
       </c>
       <c r="B83" t="s">
-        <v>345</v>
-      </c>
-      <c r="C83" t="s">
-        <v>163</v>
+        <v>372</v>
+      </c>
+      <c r="C83" s="1" t="s">
+        <v>108</v>
       </c>
       <c r="D83" t="s">
         <v>4</v>
-      </c>
-      <c r="E83" t="s">
-        <v>344</v>
       </c>
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
-        <v>258</v>
-      </c>
-      <c r="B84" t="s">
-        <v>257</v>
+        <v>65</v>
       </c>
       <c r="C84" t="s">
-        <v>163</v>
+        <v>187</v>
       </c>
       <c r="D84" t="s">
-        <v>253</v>
+        <v>4</v>
       </c>
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
-        <v>90</v>
-      </c>
-      <c r="B85" s="6" t="s">
-        <v>316</v>
-      </c>
-      <c r="C85" s="6" t="s">
-        <v>148</v>
-      </c>
-      <c r="D85" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="E85" t="s">
-        <v>318</v>
+        <v>110</v>
+      </c>
+      <c r="B85" t="s">
+        <v>309</v>
+      </c>
+      <c r="C85" t="s">
+        <v>108</v>
+      </c>
+      <c r="D85" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
-        <v>155</v>
-      </c>
-      <c r="B86">
-        <v>101</v>
+        <v>10</v>
+      </c>
+      <c r="B86" t="s">
+        <v>309</v>
       </c>
       <c r="C86" t="s">
-        <v>148</v>
+        <v>186</v>
       </c>
       <c r="D86" t="s">
         <v>4</v>
@@ -2611,93 +2803,116 @@
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
-        <v>168</v>
-      </c>
-      <c r="C87" t="s">
-        <v>163</v>
-      </c>
-      <c r="D87" t="s">
-        <v>4</v>
+        <v>280</v>
+      </c>
+      <c r="B87" s="1" t="s">
+        <v>281</v>
+      </c>
+      <c r="C87" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="D87" s="1" t="s">
+        <v>253</v>
+      </c>
+      <c r="E87" t="s">
+        <v>283</v>
       </c>
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
-        <v>326</v>
+        <v>361</v>
       </c>
       <c r="B88" t="s">
-        <v>284</v>
-      </c>
-      <c r="C88" t="s">
-        <v>148</v>
-      </c>
-      <c r="D88" t="s">
-        <v>253</v>
-      </c>
+        <v>362</v>
+      </c>
+      <c r="D88" s="5"/>
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
-        <v>165</v>
+        <v>154</v>
+      </c>
+      <c r="B89" t="s">
+        <v>309</v>
       </c>
       <c r="C89" t="s">
-        <v>163</v>
+        <v>148</v>
       </c>
       <c r="D89" t="s">
         <v>4</v>
+      </c>
+      <c r="E89" t="s">
+        <v>310</v>
       </c>
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
-        <v>128</v>
-      </c>
-      <c r="C90" t="s">
-        <v>108</v>
-      </c>
-      <c r="D90" t="s">
-        <v>4</v>
+        <v>365</v>
+      </c>
+      <c r="B90" t="s">
+        <v>328</v>
+      </c>
+      <c r="D90" s="5"/>
+      <c r="E90" t="s">
+        <v>366</v>
       </c>
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
-        <v>125</v>
+        <v>261</v>
+      </c>
+      <c r="B91" t="s">
+        <v>262</v>
       </c>
       <c r="C91" t="s">
-        <v>108</v>
+        <v>163</v>
       </c>
       <c r="D91" t="s">
-        <v>4</v>
+        <v>253</v>
       </c>
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
-        <v>123</v>
-      </c>
-      <c r="C92" t="s">
-        <v>108</v>
-      </c>
-      <c r="D92" t="s">
-        <v>4</v>
+        <v>76</v>
+      </c>
+      <c r="B92" s="2" t="s">
+        <v>309</v>
+      </c>
+      <c r="C92" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="D92" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E92" t="s">
+        <v>311</v>
       </c>
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
-        <v>121</v>
+        <v>169</v>
+      </c>
+      <c r="B93" t="s">
+        <v>338</v>
       </c>
       <c r="C93" t="s">
-        <v>108</v>
+        <v>163</v>
       </c>
       <c r="D93" t="s">
         <v>4</v>
+      </c>
+      <c r="E93" t="s">
+        <v>337</v>
       </c>
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
-        <v>254</v>
+        <v>258</v>
       </c>
       <c r="B94" t="s">
-        <v>252</v>
+        <v>257</v>
       </c>
       <c r="C94" t="s">
-        <v>108</v>
+        <v>163</v>
       </c>
       <c r="D94" t="s">
         <v>253</v>
@@ -2705,92 +2920,77 @@
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
-        <v>328</v>
-      </c>
-      <c r="B95" t="s">
-        <v>280</v>
-      </c>
-      <c r="C95" t="s">
-        <v>163</v>
-      </c>
-      <c r="D95" t="s">
-        <v>253</v>
+        <v>90</v>
+      </c>
+      <c r="B95" s="2" t="s">
+        <v>309</v>
+      </c>
+      <c r="C95" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="D95" s="2" t="s">
+        <v>4</v>
       </c>
       <c r="E95" t="s">
-        <v>334</v>
+        <v>311</v>
       </c>
     </row>
     <row r="96" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
-        <v>343</v>
-      </c>
-      <c r="B96" t="s">
-        <v>270</v>
+        <v>155</v>
+      </c>
+      <c r="B96">
+        <v>101</v>
       </c>
       <c r="C96" t="s">
-        <v>163</v>
+        <v>148</v>
       </c>
       <c r="D96" t="s">
-        <v>253</v>
-      </c>
-      <c r="E96" s="5" t="s">
-        <v>342</v>
+        <v>4</v>
       </c>
     </row>
     <row r="97" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
-        <v>341</v>
-      </c>
-      <c r="B97" t="s">
-        <v>340</v>
+        <v>168</v>
       </c>
       <c r="C97" t="s">
         <v>163</v>
       </c>
       <c r="D97" t="s">
-        <v>253</v>
-      </c>
-      <c r="E97" t="s">
-        <v>339</v>
+        <v>4</v>
       </c>
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
-        <v>331</v>
-      </c>
-      <c r="B98" t="s">
-        <v>332</v>
-      </c>
-      <c r="C98" t="s">
-        <v>108</v>
-      </c>
-      <c r="D98" t="s">
+        <v>319</v>
+      </c>
+      <c r="B98" s="1" t="s">
+        <v>278</v>
+      </c>
+      <c r="C98" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="D98" s="1" t="s">
         <v>253</v>
-      </c>
-      <c r="E98" t="s">
-        <v>333</v>
       </c>
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
-        <v>255</v>
-      </c>
-      <c r="B99" t="s">
-        <v>256</v>
+        <v>165</v>
       </c>
       <c r="C99" t="s">
-        <v>108</v>
+        <v>163</v>
       </c>
       <c r="D99" t="s">
-        <v>253</v>
+        <v>4</v>
       </c>
     </row>
     <row r="100" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
-        <v>17</v>
-      </c>
-      <c r="B100">
-        <v>0</v>
+        <v>128</v>
+      </c>
+      <c r="B100" t="s">
+        <v>373</v>
       </c>
       <c r="C100" t="s">
         <v>108</v>
@@ -2801,12 +3001,9 @@
     </row>
     <row r="101" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
-        <v>114</v>
-      </c>
-      <c r="B101">
-        <v>0</v>
-      </c>
-      <c r="C101" t="s">
+        <v>125</v>
+      </c>
+      <c r="C101" s="1" t="s">
         <v>108</v>
       </c>
       <c r="D101" t="s">
@@ -2815,10 +3012,7 @@
     </row>
     <row r="102" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
-        <v>141</v>
-      </c>
-      <c r="B102">
-        <v>0</v>
+        <v>123</v>
       </c>
       <c r="C102" t="s">
         <v>108</v>
@@ -2829,10 +3023,7 @@
     </row>
     <row r="103" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
-        <v>202</v>
-      </c>
-      <c r="B103">
-        <v>0</v>
+        <v>121</v>
       </c>
       <c r="C103" t="s">
         <v>108</v>
@@ -2843,97 +3034,109 @@
     </row>
     <row r="104" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
-        <v>59</v>
-      </c>
-      <c r="B104">
-        <v>0</v>
+        <v>254</v>
+      </c>
+      <c r="B104" t="s">
+        <v>252</v>
       </c>
       <c r="C104" t="s">
-        <v>187</v>
+        <v>108</v>
       </c>
       <c r="D104" t="s">
-        <v>4</v>
+        <v>253</v>
       </c>
     </row>
     <row r="105" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
-        <v>18</v>
-      </c>
-      <c r="B105">
-        <v>0</v>
+        <v>321</v>
+      </c>
+      <c r="B105" t="s">
+        <v>274</v>
       </c>
       <c r="C105" t="s">
-        <v>187</v>
+        <v>163</v>
       </c>
       <c r="D105" t="s">
-        <v>4</v>
+        <v>253</v>
+      </c>
+      <c r="E105" t="s">
+        <v>327</v>
       </c>
     </row>
     <row r="106" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
-        <v>197</v>
-      </c>
-      <c r="B106">
-        <v>0</v>
+        <v>336</v>
+      </c>
+      <c r="B106" t="s">
+        <v>268</v>
       </c>
       <c r="C106" t="s">
-        <v>108</v>
+        <v>163</v>
       </c>
       <c r="D106" t="s">
-        <v>4</v>
+        <v>253</v>
+      </c>
+      <c r="E106" s="4" t="s">
+        <v>335</v>
       </c>
     </row>
     <row r="107" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
-        <v>207</v>
-      </c>
-      <c r="B107">
-        <v>0</v>
+        <v>334</v>
+      </c>
+      <c r="B107" t="s">
+        <v>333</v>
       </c>
       <c r="C107" t="s">
-        <v>108</v>
+        <v>163</v>
       </c>
       <c r="D107" t="s">
-        <v>4</v>
+        <v>253</v>
+      </c>
+      <c r="E107" t="s">
+        <v>332</v>
       </c>
     </row>
     <row r="108" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
-        <v>46</v>
-      </c>
-      <c r="B108">
-        <v>0</v>
-      </c>
-      <c r="C108" s="2" t="s">
-        <v>184</v>
+        <v>324</v>
+      </c>
+      <c r="B108" t="s">
+        <v>325</v>
+      </c>
+      <c r="C108" t="s">
+        <v>108</v>
       </c>
       <c r="D108" t="s">
-        <v>4</v>
+        <v>253</v>
+      </c>
+      <c r="E108" t="s">
+        <v>326</v>
       </c>
     </row>
     <row r="109" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
-        <v>44</v>
+        <v>255</v>
       </c>
       <c r="B109" t="s">
-        <v>45</v>
+        <v>256</v>
       </c>
       <c r="C109" t="s">
-        <v>184</v>
+        <v>108</v>
       </c>
       <c r="D109" t="s">
-        <v>4</v>
+        <v>253</v>
       </c>
     </row>
     <row r="110" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
-        <v>101</v>
+        <v>17</v>
       </c>
       <c r="B110">
         <v>0</v>
       </c>
       <c r="C110" t="s">
-        <v>163</v>
+        <v>108</v>
       </c>
       <c r="D110" t="s">
         <v>4</v>
@@ -2941,7 +3144,7 @@
     </row>
     <row r="111" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
       <c r="B111">
         <v>0</v>
@@ -2955,7 +3158,7 @@
     </row>
     <row r="112" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
-        <v>209</v>
+        <v>141</v>
       </c>
       <c r="B112">
         <v>0</v>
@@ -2967,9 +3170,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="113" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
-        <v>222</v>
+        <v>202</v>
+      </c>
+      <c r="B113">
+        <v>0</v>
       </c>
       <c r="C113" t="s">
         <v>108</v>
@@ -2978,78 +3184,96 @@
         <v>4</v>
       </c>
     </row>
-    <row r="114" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
-        <v>113</v>
+        <v>59</v>
+      </c>
+      <c r="B114">
+        <v>0</v>
       </c>
       <c r="C114" t="s">
-        <v>108</v>
+        <v>187</v>
       </c>
       <c r="D114" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="115" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
-        <v>282</v>
-      </c>
-      <c r="B115" t="s">
-        <v>283</v>
+        <v>18</v>
+      </c>
+      <c r="B115">
+        <v>0</v>
+      </c>
+      <c r="C115" t="s">
+        <v>187</v>
       </c>
       <c r="D115" t="s">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="116" spans="1:5" x14ac:dyDescent="0.2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="116" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
-        <v>194</v>
+        <v>197</v>
+      </c>
+      <c r="B116">
+        <v>0</v>
       </c>
       <c r="C116" t="s">
-        <v>187</v>
+        <v>108</v>
       </c>
       <c r="D116" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="117" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
-        <v>3</v>
+        <v>207</v>
+      </c>
+      <c r="B117">
+        <v>0</v>
       </c>
       <c r="C117" t="s">
-        <v>187</v>
+        <v>108</v>
       </c>
       <c r="D117" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="118" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
-        <v>260</v>
-      </c>
-      <c r="B118" t="s">
-        <v>259</v>
-      </c>
-      <c r="C118" s="1" t="s">
-        <v>163</v>
+        <v>46</v>
+      </c>
+      <c r="B118">
+        <v>0</v>
+      </c>
+      <c r="C118" s="2" t="s">
+        <v>184</v>
       </c>
       <c r="D118" t="s">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="119" spans="1:5" x14ac:dyDescent="0.2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="119" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
-        <v>68</v>
+        <v>44</v>
+      </c>
+      <c r="B119" t="s">
+        <v>45</v>
       </c>
       <c r="C119" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="D119" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="120" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
-        <v>164</v>
+        <v>101</v>
+      </c>
+      <c r="B120">
+        <v>0</v>
       </c>
       <c r="C120" t="s">
         <v>163</v>
@@ -3058,242 +3282,221 @@
         <v>4</v>
       </c>
     </row>
-    <row r="121" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
+        <v>120</v>
+      </c>
+      <c r="B121">
+        <v>0</v>
+      </c>
+      <c r="C121" t="s">
+        <v>108</v>
+      </c>
+      <c r="D121" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="122" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A122" t="s">
+        <v>209</v>
+      </c>
+      <c r="B122">
+        <v>0</v>
+      </c>
+      <c r="C122" t="s">
+        <v>108</v>
+      </c>
+      <c r="D122" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="123" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A123" t="s">
+        <v>222</v>
+      </c>
+      <c r="C123" t="s">
+        <v>108</v>
+      </c>
+      <c r="D123" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="124" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A124" t="s">
+        <v>113</v>
+      </c>
+      <c r="C124" t="s">
+        <v>108</v>
+      </c>
+      <c r="D124" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="125" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A125" t="s">
+        <v>276</v>
+      </c>
+      <c r="B125" t="s">
+        <v>277</v>
+      </c>
+      <c r="D125" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="126" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A126" t="s">
+        <v>194</v>
+      </c>
+      <c r="C126" t="s">
+        <v>187</v>
+      </c>
+      <c r="D126" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="127" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A127" t="s">
+        <v>3</v>
+      </c>
+      <c r="C127" t="s">
+        <v>187</v>
+      </c>
+      <c r="D127" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="128" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A128" t="s">
+        <v>260</v>
+      </c>
+      <c r="B128" t="s">
+        <v>259</v>
+      </c>
+      <c r="C128" s="6" t="s">
+        <v>163</v>
+      </c>
+      <c r="D128" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="129" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A129" t="s">
+        <v>68</v>
+      </c>
+      <c r="C129" t="s">
+        <v>186</v>
+      </c>
+      <c r="D129" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="130" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A130" t="s">
+        <v>164</v>
+      </c>
+      <c r="C130" t="s">
+        <v>163</v>
+      </c>
+      <c r="D130" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="131" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A131" t="s">
         <v>104</v>
       </c>
-      <c r="B121" t="s">
-        <v>336</v>
-      </c>
-      <c r="C121" t="s">
+      <c r="B131" t="s">
+        <v>329</v>
+      </c>
+      <c r="C131" t="s">
         <v>163</v>
       </c>
-      <c r="D121" t="s">
-        <v>4</v>
-      </c>
-      <c r="E121" t="s">
+      <c r="D131" t="s">
+        <v>4</v>
+      </c>
+      <c r="E131" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="132" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A132" t="s">
+        <v>103</v>
+      </c>
+      <c r="B132" t="s">
+        <v>328</v>
+      </c>
+      <c r="C132" t="s">
+        <v>163</v>
+      </c>
+      <c r="D132" t="s">
+        <v>4</v>
+      </c>
+      <c r="E132" t="s">
         <v>330</v>
       </c>
     </row>
-    <row r="122" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A122" t="s">
-        <v>103</v>
-      </c>
-      <c r="B122" t="s">
-        <v>335</v>
-      </c>
-      <c r="C122" t="s">
-        <v>163</v>
-      </c>
-      <c r="D122" t="s">
-        <v>4</v>
-      </c>
-      <c r="E122" t="s">
-        <v>337</v>
-      </c>
-    </row>
-    <row r="123" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A123" t="s">
+    <row r="133" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A133" t="s">
         <v>144</v>
       </c>
-      <c r="B123">
+      <c r="B133">
         <v>153</v>
       </c>
-      <c r="C123" t="s">
-        <v>108</v>
-      </c>
-      <c r="D123" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="124" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A124" t="s">
+      <c r="C133" t="s">
+        <v>108</v>
+      </c>
+      <c r="D133" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="134" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A134" t="s">
         <v>19</v>
       </c>
-      <c r="B124">
+      <c r="B134">
         <v>331</v>
       </c>
-      <c r="C124" t="s">
+      <c r="C134" t="s">
         <v>186</v>
       </c>
-      <c r="D124" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="125" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A125" t="s">
+      <c r="D134" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="135" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A135" t="s">
         <v>192</v>
       </c>
-      <c r="B125" s="1">
+      <c r="B135" s="6">
         <v>106</v>
       </c>
-      <c r="C125" s="1" t="s">
+      <c r="C135" s="6" t="s">
         <v>187</v>
       </c>
-      <c r="D125" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="126" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A126" t="s">
+      <c r="D135" s="6" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="136" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A136" t="s">
         <v>208</v>
       </c>
-      <c r="B126">
+      <c r="B136">
         <v>123</v>
       </c>
-      <c r="C126" t="s">
-        <v>108</v>
-      </c>
-      <c r="D126" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="127" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A127" t="s">
+      <c r="C136" t="s">
+        <v>108</v>
+      </c>
+      <c r="D136" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="137" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A137" t="s">
         <v>14</v>
       </c>
-      <c r="B127">
+      <c r="B137">
         <v>195</v>
-      </c>
-      <c r="C127" t="s">
-        <v>186</v>
-      </c>
-      <c r="D127" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="128" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A128" t="s">
-        <v>204</v>
-      </c>
-      <c r="B128">
-        <v>434</v>
-      </c>
-      <c r="C128" t="s">
-        <v>108</v>
-      </c>
-      <c r="D128" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="129" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A129" t="s">
-        <v>203</v>
-      </c>
-      <c r="B129">
-        <v>223</v>
-      </c>
-      <c r="C129" t="s">
-        <v>108</v>
-      </c>
-      <c r="D129" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="130" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A130" t="s">
-        <v>196</v>
-      </c>
-      <c r="B130">
-        <v>223</v>
-      </c>
-      <c r="C130" t="s">
-        <v>108</v>
-      </c>
-      <c r="D130" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="131" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A131" t="s">
-        <v>145</v>
-      </c>
-      <c r="B131">
-        <v>223</v>
-      </c>
-      <c r="C131" t="s">
-        <v>108</v>
-      </c>
-      <c r="D131" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="132" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A132" t="s">
-        <v>53</v>
-      </c>
-      <c r="B132">
-        <v>153</v>
-      </c>
-      <c r="C132" t="s">
-        <v>184</v>
-      </c>
-      <c r="D132" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="133" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A133" t="s">
-        <v>40</v>
-      </c>
-      <c r="B133">
-        <v>332</v>
-      </c>
-      <c r="C133" t="s">
-        <v>186</v>
-      </c>
-      <c r="D133" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="134" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A134" t="s">
-        <v>142</v>
-      </c>
-      <c r="B134" t="s">
-        <v>143</v>
-      </c>
-      <c r="C134" t="s">
-        <v>108</v>
-      </c>
-      <c r="D134" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="135" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A135" t="s">
-        <v>15</v>
-      </c>
-      <c r="B135">
-        <v>102</v>
-      </c>
-      <c r="C135" t="s">
-        <v>186</v>
-      </c>
-      <c r="D135" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="136" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A136" t="s">
-        <v>39</v>
-      </c>
-      <c r="B136">
-        <v>471</v>
-      </c>
-      <c r="C136" t="s">
-        <v>186</v>
-      </c>
-      <c r="D136" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="137" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A137" t="s">
-        <v>24</v>
-      </c>
-      <c r="B137">
-        <v>331</v>
       </c>
       <c r="C137" t="s">
         <v>186</v>
@@ -3302,26 +3505,26 @@
         <v>4</v>
       </c>
     </row>
-    <row r="138" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A138" t="s">
-        <v>217</v>
-      </c>
-      <c r="B138" s="1">
-        <v>104</v>
-      </c>
-      <c r="C138" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="D138" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="139" spans="1:4" x14ac:dyDescent="0.2">
+        <v>204</v>
+      </c>
+      <c r="B138">
+        <v>434</v>
+      </c>
+      <c r="C138" t="s">
+        <v>108</v>
+      </c>
+      <c r="D138" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="139" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A139" t="s">
-        <v>109</v>
+        <v>203</v>
       </c>
       <c r="B139">
-        <v>753</v>
+        <v>223</v>
       </c>
       <c r="C139" t="s">
         <v>108</v>
@@ -3330,12 +3533,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="140" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A140" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="B140">
-        <v>128</v>
+        <v>223</v>
       </c>
       <c r="C140" t="s">
         <v>108</v>
@@ -3344,57 +3547,57 @@
         <v>4</v>
       </c>
     </row>
-    <row r="141" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A141" t="s">
-        <v>13</v>
+        <v>145</v>
       </c>
       <c r="B141">
-        <v>272</v>
+        <v>223</v>
       </c>
       <c r="C141" t="s">
+        <v>108</v>
+      </c>
+      <c r="D141" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="142" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A142" t="s">
+        <v>53</v>
+      </c>
+      <c r="B142">
+        <v>153</v>
+      </c>
+      <c r="C142" t="s">
+        <v>184</v>
+      </c>
+      <c r="D142" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="143" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A143" t="s">
+        <v>40</v>
+      </c>
+      <c r="B143">
+        <v>332</v>
+      </c>
+      <c r="C143" t="s">
         <v>186</v>
       </c>
-      <c r="D141" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="142" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A142" t="s">
-        <v>56</v>
-      </c>
-      <c r="B142">
-        <v>471</v>
-      </c>
-      <c r="C142" s="1" t="s">
-        <v>187</v>
-      </c>
-      <c r="D142" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="143" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A143" t="s">
-        <v>64</v>
-      </c>
-      <c r="B143">
-        <v>193</v>
-      </c>
-      <c r="C143" t="s">
-        <v>187</v>
-      </c>
       <c r="D143" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="144" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="144" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A144" t="s">
-        <v>32</v>
-      </c>
-      <c r="B144">
-        <v>321</v>
+        <v>142</v>
+      </c>
+      <c r="B144" t="s">
+        <v>143</v>
       </c>
       <c r="C144" t="s">
-        <v>187</v>
+        <v>108</v>
       </c>
       <c r="D144" t="s">
         <v>4</v>
@@ -3402,13 +3605,13 @@
     </row>
     <row r="145" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A145" t="s">
-        <v>199</v>
+        <v>15</v>
       </c>
       <c r="B145">
-        <v>151</v>
+        <v>102</v>
       </c>
       <c r="C145" t="s">
-        <v>108</v>
+        <v>186</v>
       </c>
       <c r="D145" t="s">
         <v>4</v>
@@ -3416,13 +3619,13 @@
     </row>
     <row r="146" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A146" t="s">
-        <v>189</v>
+        <v>39</v>
       </c>
       <c r="B146">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="C146" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D146" t="s">
         <v>4</v>
@@ -3430,13 +3633,13 @@
     </row>
     <row r="147" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A147" t="s">
-        <v>62</v>
-      </c>
-      <c r="B147" t="s">
-        <v>63</v>
+        <v>24</v>
+      </c>
+      <c r="B147">
+        <v>331</v>
       </c>
       <c r="C147" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D147" t="s">
         <v>4</v>
@@ -3444,24 +3647,27 @@
     </row>
     <row r="148" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A148" t="s">
-        <v>214</v>
-      </c>
-      <c r="B148">
-        <v>223</v>
-      </c>
-      <c r="C148" t="s">
-        <v>108</v>
-      </c>
-      <c r="D148" t="s">
+        <v>217</v>
+      </c>
+      <c r="B148" s="6">
+        <v>104</v>
+      </c>
+      <c r="C148" s="6" t="s">
+        <v>108</v>
+      </c>
+      <c r="D148" s="6" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="149" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A149" t="s">
-        <v>55</v>
-      </c>
-      <c r="C149" s="2" t="s">
-        <v>187</v>
+        <v>109</v>
+      </c>
+      <c r="B149">
+        <v>753</v>
+      </c>
+      <c r="C149" t="s">
+        <v>108</v>
       </c>
       <c r="D149" t="s">
         <v>4</v>
@@ -3469,13 +3675,13 @@
     </row>
     <row r="150" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A150" t="s">
-        <v>9</v>
+        <v>198</v>
       </c>
       <c r="B150">
-        <v>471</v>
+        <v>128</v>
       </c>
       <c r="C150" t="s">
-        <v>186</v>
+        <v>108</v>
       </c>
       <c r="D150" t="s">
         <v>4</v>
@@ -3483,10 +3689,10 @@
     </row>
     <row r="151" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A151" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="B151">
-        <v>180</v>
+        <v>272</v>
       </c>
       <c r="C151" t="s">
         <v>186</v>
@@ -3497,13 +3703,13 @@
     </row>
     <row r="152" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A152" t="s">
-        <v>16</v>
+        <v>56</v>
       </c>
       <c r="B152">
         <v>471</v>
       </c>
-      <c r="C152" t="s">
-        <v>186</v>
+      <c r="C152" s="6" t="s">
+        <v>187</v>
       </c>
       <c r="D152" t="s">
         <v>4</v>
@@ -3511,10 +3717,10 @@
     </row>
     <row r="153" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A153" t="s">
-        <v>33</v>
+        <v>64</v>
       </c>
       <c r="B153">
-        <v>401</v>
+        <v>193</v>
       </c>
       <c r="C153" t="s">
         <v>187</v>
@@ -3525,10 +3731,10 @@
     </row>
     <row r="154" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A154" t="s">
-        <v>57</v>
+        <v>32</v>
       </c>
       <c r="B154">
-        <v>302</v>
+        <v>321</v>
       </c>
       <c r="C154" t="s">
         <v>187</v>
@@ -3539,13 +3745,13 @@
     </row>
     <row r="155" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A155" t="s">
-        <v>5</v>
+        <v>199</v>
       </c>
       <c r="B155">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="C155" t="s">
-        <v>187</v>
+        <v>108</v>
       </c>
       <c r="D155" t="s">
         <v>4</v>
@@ -3553,10 +3759,13 @@
     </row>
     <row r="156" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A156" t="s">
-        <v>220</v>
+        <v>189</v>
+      </c>
+      <c r="B156">
+        <v>472</v>
       </c>
       <c r="C156" t="s">
-        <v>108</v>
+        <v>187</v>
       </c>
       <c r="D156" t="s">
         <v>4</v>
@@ -3564,13 +3773,13 @@
     </row>
     <row r="157" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A157" t="s">
-        <v>27</v>
-      </c>
-      <c r="B157">
-        <v>154</v>
+        <v>62</v>
+      </c>
+      <c r="B157" t="s">
+        <v>63</v>
       </c>
       <c r="C157" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="D157" t="s">
         <v>4</v>
@@ -3578,10 +3787,10 @@
     </row>
     <row r="158" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A158" t="s">
-        <v>35</v>
+        <v>214</v>
       </c>
       <c r="B158">
-        <v>392</v>
+        <v>223</v>
       </c>
       <c r="C158" t="s">
         <v>108</v>
@@ -3592,13 +3801,10 @@
     </row>
     <row r="159" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A159" t="s">
-        <v>25</v>
-      </c>
-      <c r="B159">
-        <v>220</v>
-      </c>
-      <c r="C159" t="s">
-        <v>186</v>
+        <v>55</v>
+      </c>
+      <c r="C159" s="2" t="s">
+        <v>187</v>
       </c>
       <c r="D159" t="s">
         <v>4</v>
@@ -3606,13 +3812,13 @@
     </row>
     <row r="160" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A160" t="s">
-        <v>31</v>
+        <v>9</v>
       </c>
       <c r="B160">
-        <v>295</v>
+        <v>471</v>
       </c>
       <c r="C160" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D160" t="s">
         <v>4</v>
@@ -3620,10 +3826,10 @@
     </row>
     <row r="161" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A161" t="s">
-        <v>22</v>
+        <v>8</v>
       </c>
       <c r="B161">
-        <v>223</v>
+        <v>180</v>
       </c>
       <c r="C161" t="s">
         <v>186</v>
@@ -3634,10 +3840,10 @@
     </row>
     <row r="162" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A162" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="B162">
-        <v>223</v>
+        <v>471</v>
       </c>
       <c r="C162" t="s">
         <v>186</v>
@@ -3648,13 +3854,13 @@
     </row>
     <row r="163" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A163" t="s">
-        <v>213</v>
-      </c>
-      <c r="B163" t="s">
-        <v>215</v>
+        <v>33</v>
+      </c>
+      <c r="B163">
+        <v>401</v>
       </c>
       <c r="C163" t="s">
-        <v>108</v>
+        <v>187</v>
       </c>
       <c r="D163" t="s">
         <v>4</v>
@@ -3662,10 +3868,10 @@
     </row>
     <row r="164" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A164" t="s">
-        <v>58</v>
-      </c>
-      <c r="B164" t="s">
-        <v>60</v>
+        <v>57</v>
+      </c>
+      <c r="B164">
+        <v>302</v>
       </c>
       <c r="C164" t="s">
         <v>187</v>
@@ -3676,10 +3882,10 @@
     </row>
     <row r="165" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A165" t="s">
-        <v>61</v>
+        <v>5</v>
       </c>
       <c r="B165">
-        <v>393</v>
+        <v>153</v>
       </c>
       <c r="C165" t="s">
         <v>187</v>
@@ -3690,13 +3896,10 @@
     </row>
     <row r="166" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A166" t="s">
-        <v>7</v>
-      </c>
-      <c r="B166">
-        <v>105</v>
+        <v>220</v>
       </c>
       <c r="C166" t="s">
-        <v>187</v>
+        <v>108</v>
       </c>
       <c r="D166" t="s">
         <v>4</v>
@@ -3704,13 +3907,13 @@
     </row>
     <row r="167" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A167" t="s">
-        <v>28</v>
-      </c>
-      <c r="B167" t="s">
-        <v>29</v>
+        <v>27</v>
+      </c>
+      <c r="B167">
+        <v>154</v>
       </c>
       <c r="C167" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D167" t="s">
         <v>4</v>
@@ -3718,10 +3921,10 @@
     </row>
     <row r="168" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A168" t="s">
-        <v>139</v>
+        <v>35</v>
       </c>
       <c r="B168">
-        <v>102</v>
+        <v>392</v>
       </c>
       <c r="C168" t="s">
         <v>108</v>
@@ -3732,13 +3935,13 @@
     </row>
     <row r="169" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A169" t="s">
-        <v>140</v>
+        <v>25</v>
       </c>
       <c r="B169">
-        <v>474</v>
+        <v>220</v>
       </c>
       <c r="C169" t="s">
-        <v>108</v>
+        <v>186</v>
       </c>
       <c r="D169" t="s">
         <v>4</v>
@@ -3746,13 +3949,13 @@
     </row>
     <row r="170" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A170" t="s">
-        <v>20</v>
+        <v>31</v>
       </c>
       <c r="B170">
-        <v>392</v>
+        <v>295</v>
       </c>
       <c r="C170" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="D170" t="s">
         <v>4</v>
@@ -3760,13 +3963,13 @@
     </row>
     <row r="171" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A171" t="s">
-        <v>195</v>
+        <v>22</v>
       </c>
       <c r="B171">
-        <v>514</v>
+        <v>223</v>
       </c>
       <c r="C171" t="s">
-        <v>108</v>
+        <v>186</v>
       </c>
       <c r="D171" t="s">
         <v>4</v>
@@ -3774,13 +3977,13 @@
     </row>
     <row r="172" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A172" t="s">
-        <v>191</v>
+        <v>21</v>
       </c>
       <c r="B172">
-        <v>514</v>
+        <v>223</v>
       </c>
       <c r="C172" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D172" t="s">
         <v>4</v>
@@ -3788,13 +3991,13 @@
     </row>
     <row r="173" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A173" t="s">
-        <v>36</v>
-      </c>
-      <c r="B173">
-        <v>105</v>
+        <v>213</v>
+      </c>
+      <c r="B173" t="s">
+        <v>215</v>
       </c>
       <c r="C173" t="s">
-        <v>187</v>
+        <v>108</v>
       </c>
       <c r="D173" t="s">
         <v>4</v>
@@ -3802,13 +4005,13 @@
     </row>
     <row r="174" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A174" t="s">
-        <v>212</v>
-      </c>
-      <c r="B174">
-        <v>103</v>
+        <v>58</v>
+      </c>
+      <c r="B174" t="s">
+        <v>60</v>
       </c>
       <c r="C174" t="s">
-        <v>108</v>
+        <v>187</v>
       </c>
       <c r="D174" t="s">
         <v>4</v>
@@ -3816,13 +4019,13 @@
     </row>
     <row r="175" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A175" t="s">
-        <v>26</v>
+        <v>61</v>
       </c>
       <c r="B175">
-        <v>470</v>
+        <v>393</v>
       </c>
       <c r="C175" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="D175" t="s">
         <v>4</v>
@@ -3830,10 +4033,10 @@
     </row>
     <row r="176" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A176" t="s">
-        <v>38</v>
+        <v>7</v>
       </c>
       <c r="B176">
-        <v>514</v>
+        <v>105</v>
       </c>
       <c r="C176" t="s">
         <v>187</v>
@@ -3844,13 +4047,13 @@
     </row>
     <row r="177" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A177" t="s">
-        <v>41</v>
-      </c>
-      <c r="B177">
-        <v>295</v>
+        <v>28</v>
+      </c>
+      <c r="B177" t="s">
+        <v>29</v>
       </c>
       <c r="C177" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="D177" t="s">
         <v>4</v>
@@ -3858,13 +4061,13 @@
     </row>
     <row r="178" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A178" t="s">
-        <v>30</v>
+        <v>139</v>
       </c>
       <c r="B178">
-        <v>471</v>
+        <v>102</v>
       </c>
       <c r="C178" t="s">
-        <v>187</v>
+        <v>108</v>
       </c>
       <c r="D178" t="s">
         <v>4</v>
@@ -3872,13 +4075,13 @@
     </row>
     <row r="179" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A179" t="s">
-        <v>43</v>
+        <v>140</v>
       </c>
       <c r="B179">
-        <v>103</v>
+        <v>474</v>
       </c>
       <c r="C179" t="s">
-        <v>186</v>
+        <v>108</v>
       </c>
       <c r="D179" t="s">
         <v>4</v>
@@ -3886,13 +4089,13 @@
     </row>
     <row r="180" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A180" t="s">
-        <v>211</v>
+        <v>20</v>
       </c>
       <c r="B180">
-        <v>103</v>
+        <v>392</v>
       </c>
       <c r="C180" t="s">
-        <v>108</v>
+        <v>186</v>
       </c>
       <c r="D180" t="s">
         <v>4</v>
@@ -3900,13 +4103,13 @@
     </row>
     <row r="181" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A181" t="s">
-        <v>42</v>
+        <v>195</v>
       </c>
       <c r="B181">
-        <v>683</v>
+        <v>514</v>
       </c>
       <c r="C181" t="s">
-        <v>186</v>
+        <v>108</v>
       </c>
       <c r="D181" t="s">
         <v>4</v>
@@ -3914,13 +4117,13 @@
     </row>
     <row r="182" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A182" t="s">
-        <v>236</v>
+        <v>191</v>
       </c>
       <c r="B182">
-        <v>472</v>
+        <v>514</v>
       </c>
       <c r="C182" t="s">
-        <v>108</v>
+        <v>187</v>
       </c>
       <c r="D182" t="s">
         <v>4</v>
@@ -3928,13 +4131,13 @@
     </row>
     <row r="183" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A183" t="s">
-        <v>210</v>
+        <v>36</v>
       </c>
       <c r="B183">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="C183" t="s">
-        <v>108</v>
+        <v>187</v>
       </c>
       <c r="D183" t="s">
         <v>4</v>
@@ -3942,10 +4145,13 @@
     </row>
     <row r="184" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A184" t="s">
-        <v>193</v>
+        <v>212</v>
+      </c>
+      <c r="B184">
+        <v>103</v>
       </c>
       <c r="C184" t="s">
-        <v>187</v>
+        <v>108</v>
       </c>
       <c r="D184" t="s">
         <v>4</v>
@@ -3953,30 +4159,27 @@
     </row>
     <row r="185" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A185" t="s">
-        <v>291</v>
-      </c>
-      <c r="B185" t="s">
-        <v>292</v>
+        <v>26</v>
+      </c>
+      <c r="B185">
+        <v>470</v>
       </c>
       <c r="C185" t="s">
-        <v>148</v>
+        <v>186</v>
       </c>
       <c r="D185" t="s">
-        <v>253</v>
-      </c>
-      <c r="E185" t="s">
-        <v>313</v>
+        <v>4</v>
       </c>
     </row>
     <row r="186" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A186" t="s">
-        <v>86</v>
+        <v>38</v>
       </c>
       <c r="B186">
-        <v>101</v>
+        <v>514</v>
       </c>
       <c r="C186" t="s">
-        <v>148</v>
+        <v>187</v>
       </c>
       <c r="D186" t="s">
         <v>4</v>
@@ -3984,13 +4187,13 @@
     </row>
     <row r="187" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A187" t="s">
-        <v>91</v>
-      </c>
-      <c r="B187" t="s">
-        <v>183</v>
+        <v>41</v>
+      </c>
+      <c r="B187">
+        <v>295</v>
       </c>
       <c r="C187" t="s">
-        <v>148</v>
+        <v>186</v>
       </c>
       <c r="D187" t="s">
         <v>4</v>
@@ -3998,27 +4201,27 @@
     </row>
     <row r="188" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A188" t="s">
-        <v>321</v>
-      </c>
-      <c r="B188" t="s">
-        <v>309</v>
+        <v>30</v>
+      </c>
+      <c r="B188">
+        <v>471</v>
       </c>
       <c r="C188" t="s">
-        <v>148</v>
+        <v>187</v>
       </c>
       <c r="D188" t="s">
-        <v>253</v>
+        <v>4</v>
       </c>
     </row>
     <row r="189" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A189" t="s">
-        <v>92</v>
+        <v>43</v>
       </c>
       <c r="B189">
-        <v>470</v>
+        <v>103</v>
       </c>
       <c r="C189" t="s">
-        <v>148</v>
+        <v>186</v>
       </c>
       <c r="D189" t="s">
         <v>4</v>
@@ -4026,27 +4229,30 @@
     </row>
     <row r="190" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A190" t="s">
-        <v>320</v>
+        <v>211</v>
       </c>
       <c r="B190" t="s">
-        <v>310</v>
+        <v>370</v>
       </c>
       <c r="C190" t="s">
-        <v>148</v>
+        <v>108</v>
       </c>
       <c r="D190" t="s">
-        <v>253</v>
+        <v>4</v>
+      </c>
+      <c r="E190" t="s">
+        <v>375</v>
       </c>
     </row>
     <row r="191" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A191" t="s">
-        <v>88</v>
+        <v>42</v>
       </c>
       <c r="B191">
-        <v>182</v>
+        <v>683</v>
       </c>
       <c r="C191" t="s">
-        <v>148</v>
+        <v>186</v>
       </c>
       <c r="D191" t="s">
         <v>4</v>
@@ -4054,64 +4260,66 @@
     </row>
     <row r="192" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A192" t="s">
-        <v>152</v>
+        <v>236</v>
+      </c>
+      <c r="B192">
+        <v>472</v>
       </c>
       <c r="C192" t="s">
-        <v>148</v>
+        <v>108</v>
       </c>
       <c r="D192" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="193" spans="1:5" ht="18" x14ac:dyDescent="0.2">
+    <row r="193" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A193" t="s">
-        <v>301</v>
-      </c>
-      <c r="B193" t="s">
-        <v>302</v>
+        <v>210</v>
+      </c>
+      <c r="B193">
+        <v>104</v>
       </c>
       <c r="C193" t="s">
-        <v>148</v>
+        <v>108</v>
       </c>
       <c r="D193" t="s">
-        <v>253</v>
-      </c>
-      <c r="E193" s="4"/>
+        <v>4</v>
+      </c>
     </row>
     <row r="194" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A194" t="s">
-        <v>322</v>
-      </c>
-      <c r="B194" t="s">
-        <v>308</v>
+        <v>193</v>
       </c>
       <c r="C194" t="s">
-        <v>148</v>
+        <v>187</v>
       </c>
       <c r="D194" t="s">
-        <v>253</v>
+        <v>4</v>
       </c>
     </row>
     <row r="195" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A195" t="s">
-        <v>150</v>
-      </c>
-      <c r="B195">
-        <v>153</v>
+        <v>284</v>
+      </c>
+      <c r="B195" t="s">
+        <v>285</v>
       </c>
       <c r="C195" t="s">
         <v>148</v>
       </c>
       <c r="D195" t="s">
-        <v>4</v>
+        <v>253</v>
+      </c>
+      <c r="E195" t="s">
+        <v>306</v>
       </c>
     </row>
     <row r="196" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A196" t="s">
-        <v>157</v>
-      </c>
-      <c r="B196" t="s">
-        <v>63</v>
+        <v>86</v>
+      </c>
+      <c r="B196">
+        <v>101</v>
       </c>
       <c r="C196" t="s">
         <v>148</v>
@@ -4122,24 +4330,27 @@
     </row>
     <row r="197" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A197" t="s">
-        <v>79</v>
+        <v>346</v>
       </c>
       <c r="B197" t="s">
-        <v>80</v>
+        <v>348</v>
       </c>
       <c r="C197" t="s">
         <v>148</v>
       </c>
       <c r="D197" t="s">
-        <v>4</v>
+        <v>253</v>
+      </c>
+      <c r="E197" t="s">
+        <v>347</v>
       </c>
     </row>
     <row r="198" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A198" t="s">
-        <v>162</v>
-      </c>
-      <c r="B198">
-        <v>103</v>
+        <v>91</v>
+      </c>
+      <c r="B198" t="s">
+        <v>183</v>
       </c>
       <c r="C198" t="s">
         <v>148</v>
@@ -4150,38 +4361,38 @@
     </row>
     <row r="199" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A199" t="s">
-        <v>151</v>
-      </c>
-      <c r="B199">
-        <v>472</v>
+        <v>314</v>
+      </c>
+      <c r="B199" t="s">
+        <v>302</v>
       </c>
       <c r="C199" t="s">
         <v>148</v>
       </c>
       <c r="D199" t="s">
-        <v>4</v>
+        <v>253</v>
       </c>
     </row>
     <row r="200" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A200" t="s">
-        <v>159</v>
-      </c>
-      <c r="B200" t="s">
-        <v>160</v>
-      </c>
-      <c r="C200" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="B200">
+        <v>470</v>
+      </c>
+      <c r="C200" t="s">
         <v>148</v>
       </c>
       <c r="D200" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="201" spans="1:5" ht="18" x14ac:dyDescent="0.2">
+    <row r="201" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A201" t="s">
+        <v>313</v>
+      </c>
+      <c r="B201" t="s">
         <v>303</v>
-      </c>
-      <c r="B201" t="s">
-        <v>305</v>
       </c>
       <c r="C201" t="s">
         <v>148</v>
@@ -4189,73 +4400,70 @@
       <c r="D201" t="s">
         <v>253</v>
       </c>
-      <c r="E201" s="4"/>
     </row>
     <row r="202" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A202" t="s">
-        <v>304</v>
-      </c>
-      <c r="B202" t="s">
-        <v>305</v>
+        <v>88</v>
+      </c>
+      <c r="B202">
+        <v>182</v>
       </c>
       <c r="C202" t="s">
         <v>148</v>
       </c>
       <c r="D202" t="s">
-        <v>253</v>
+        <v>4</v>
       </c>
     </row>
     <row r="203" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A203" t="s">
-        <v>178</v>
-      </c>
-      <c r="B203">
-        <v>189</v>
+        <v>152</v>
       </c>
       <c r="C203" t="s">
-        <v>163</v>
+        <v>148</v>
       </c>
       <c r="D203" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="204" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="204" spans="1:5" ht="18" x14ac:dyDescent="0.2">
       <c r="A204" t="s">
-        <v>180</v>
-      </c>
-      <c r="B204">
-        <v>203</v>
+        <v>294</v>
+      </c>
+      <c r="B204" t="s">
+        <v>295</v>
       </c>
       <c r="C204" t="s">
-        <v>163</v>
+        <v>148</v>
       </c>
       <c r="D204" t="s">
-        <v>4</v>
-      </c>
+        <v>253</v>
+      </c>
+      <c r="E204" s="3"/>
     </row>
     <row r="205" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A205" t="s">
-        <v>87</v>
-      </c>
-      <c r="B205">
-        <v>471</v>
+        <v>315</v>
+      </c>
+      <c r="B205" t="s">
+        <v>301</v>
       </c>
       <c r="C205" t="s">
         <v>148</v>
       </c>
       <c r="D205" t="s">
-        <v>4</v>
+        <v>253</v>
       </c>
     </row>
     <row r="206" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A206" t="s">
-        <v>176</v>
+        <v>150</v>
       </c>
       <c r="B206">
-        <v>10001</v>
+        <v>153</v>
       </c>
       <c r="C206" t="s">
-        <v>163</v>
+        <v>148</v>
       </c>
       <c r="D206" t="s">
         <v>4</v>
@@ -4263,13 +4471,13 @@
     </row>
     <row r="207" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A207" t="s">
-        <v>175</v>
-      </c>
-      <c r="B207">
-        <v>202</v>
+        <v>157</v>
+      </c>
+      <c r="B207" t="s">
+        <v>63</v>
       </c>
       <c r="C207" t="s">
-        <v>163</v>
+        <v>148</v>
       </c>
       <c r="D207" t="s">
         <v>4</v>
@@ -4277,94 +4485,98 @@
     </row>
     <row r="208" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A208" t="s">
-        <v>174</v>
-      </c>
-      <c r="B208">
-        <v>471</v>
+        <v>79</v>
+      </c>
+      <c r="B208" t="s">
+        <v>80</v>
       </c>
       <c r="C208" t="s">
-        <v>163</v>
+        <v>148</v>
       </c>
       <c r="D208" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="209" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E208" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="209" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A209" t="s">
-        <v>99</v>
+        <v>162</v>
       </c>
       <c r="B209">
-        <v>202</v>
+        <v>103</v>
       </c>
       <c r="C209" t="s">
-        <v>163</v>
+        <v>148</v>
       </c>
       <c r="D209" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="210" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="210" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A210" t="s">
-        <v>98</v>
+        <v>151</v>
       </c>
       <c r="B210">
-        <v>4701</v>
+        <v>472</v>
       </c>
       <c r="C210" t="s">
-        <v>163</v>
+        <v>148</v>
       </c>
       <c r="D210" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="211" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="211" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A211" t="s">
-        <v>105</v>
-      </c>
-      <c r="B211">
-        <v>103</v>
+        <v>159</v>
+      </c>
+      <c r="B211" t="s">
+        <v>160</v>
       </c>
       <c r="C211" t="s">
-        <v>163</v>
+        <v>148</v>
       </c>
       <c r="D211" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="212" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="212" spans="1:5" ht="18" x14ac:dyDescent="0.2">
       <c r="A212" t="s">
-        <v>97</v>
-      </c>
-      <c r="B212">
-        <v>102</v>
+        <v>296</v>
+      </c>
+      <c r="B212" t="s">
+        <v>298</v>
       </c>
       <c r="C212" t="s">
-        <v>163</v>
+        <v>148</v>
       </c>
       <c r="D212" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="213" spans="1:4" x14ac:dyDescent="0.2">
+        <v>253</v>
+      </c>
+      <c r="E212" s="3"/>
+    </row>
+    <row r="213" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A213" t="s">
-        <v>172</v>
+        <v>297</v>
       </c>
       <c r="B213" t="s">
-        <v>173</v>
+        <v>298</v>
       </c>
       <c r="C213" t="s">
-        <v>163</v>
+        <v>148</v>
       </c>
       <c r="D213" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="214" spans="1:4" x14ac:dyDescent="0.2">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="214" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A214" t="s">
-        <v>71</v>
+        <v>178</v>
       </c>
       <c r="B214">
-        <v>202</v>
+        <v>189</v>
       </c>
       <c r="C214" t="s">
         <v>163</v>
@@ -4373,26 +4585,26 @@
         <v>4</v>
       </c>
     </row>
-    <row r="215" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="215" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A215" t="s">
-        <v>89</v>
+        <v>180</v>
       </c>
       <c r="B215">
+        <v>203</v>
+      </c>
+      <c r="C215" t="s">
+        <v>163</v>
+      </c>
+      <c r="D215" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="216" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A216" t="s">
+        <v>87</v>
+      </c>
+      <c r="B216">
         <v>471</v>
-      </c>
-      <c r="C215" t="s">
-        <v>148</v>
-      </c>
-      <c r="D215" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="216" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A216" t="s">
-        <v>84</v>
-      </c>
-      <c r="B216">
-        <v>103</v>
       </c>
       <c r="C216" t="s">
         <v>148</v>
@@ -4401,26 +4613,26 @@
         <v>4</v>
       </c>
     </row>
-    <row r="217" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="217" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A217" t="s">
-        <v>74</v>
+        <v>176</v>
       </c>
       <c r="B217">
-        <v>470</v>
+        <v>10001</v>
       </c>
       <c r="C217" t="s">
-        <v>148</v>
+        <v>163</v>
       </c>
       <c r="D217" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="218" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="218" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A218" t="s">
-        <v>70</v>
+        <v>175</v>
       </c>
       <c r="B218">
-        <v>472</v>
+        <v>202</v>
       </c>
       <c r="C218" t="s">
         <v>163</v>
@@ -4429,26 +4641,26 @@
         <v>4</v>
       </c>
     </row>
-    <row r="219" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="219" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A219" t="s">
-        <v>73</v>
+        <v>174</v>
       </c>
       <c r="B219">
-        <v>289</v>
+        <v>471</v>
       </c>
       <c r="C219" t="s">
-        <v>148</v>
+        <v>163</v>
       </c>
       <c r="D219" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="220" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="220" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A220" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B220">
-        <v>101</v>
+        <v>202</v>
       </c>
       <c r="C220" t="s">
         <v>163</v>
@@ -4457,12 +4669,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="221" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="221" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A221" t="s">
-        <v>69</v>
+        <v>98</v>
       </c>
       <c r="B221">
-        <v>103</v>
+        <v>4701</v>
       </c>
       <c r="C221" t="s">
         <v>163</v>
@@ -4471,12 +4683,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="222" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="222" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A222" t="s">
-        <v>96</v>
+        <v>105</v>
       </c>
       <c r="B222">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="C222" t="s">
         <v>163</v>
@@ -4485,29 +4697,29 @@
         <v>4</v>
       </c>
     </row>
-    <row r="223" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="223" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A223" t="s">
-        <v>77</v>
+        <v>97</v>
       </c>
       <c r="B223">
-        <v>0</v>
+        <v>102</v>
       </c>
       <c r="C223" t="s">
-        <v>148</v>
+        <v>163</v>
       </c>
       <c r="D223" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="224" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="224" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A224" t="s">
-        <v>75</v>
-      </c>
-      <c r="B224">
-        <v>4531</v>
+        <v>172</v>
+      </c>
+      <c r="B224" t="s">
+        <v>173</v>
       </c>
       <c r="C224" t="s">
-        <v>148</v>
+        <v>163</v>
       </c>
       <c r="D224" t="s">
         <v>4</v>
@@ -4515,13 +4727,13 @@
     </row>
     <row r="225" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A225" t="s">
-        <v>82</v>
-      </c>
-      <c r="B225" t="s">
-        <v>45</v>
+        <v>71</v>
+      </c>
+      <c r="B225">
+        <v>202</v>
       </c>
       <c r="C225" t="s">
-        <v>148</v>
+        <v>163</v>
       </c>
       <c r="D225" t="s">
         <v>4</v>
@@ -4529,13 +4741,13 @@
     </row>
     <row r="226" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A226" t="s">
-        <v>67</v>
+        <v>89</v>
       </c>
       <c r="B226">
-        <v>203</v>
+        <v>471</v>
       </c>
       <c r="C226" t="s">
-        <v>186</v>
+        <v>148</v>
       </c>
       <c r="D226" t="s">
         <v>4</v>
@@ -4543,13 +4755,13 @@
     </row>
     <row r="227" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A227" t="s">
-        <v>66</v>
+        <v>84</v>
       </c>
       <c r="B227">
-        <v>203</v>
+        <v>103</v>
       </c>
       <c r="C227" t="s">
-        <v>186</v>
+        <v>148</v>
       </c>
       <c r="D227" t="s">
         <v>4</v>
@@ -4557,42 +4769,41 @@
     </row>
     <row r="228" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A228" t="s">
-        <v>323</v>
-      </c>
-      <c r="B228" t="s">
-        <v>307</v>
+        <v>74</v>
+      </c>
+      <c r="B228">
+        <v>470</v>
       </c>
       <c r="C228" t="s">
         <v>148</v>
       </c>
       <c r="D228" t="s">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="229" spans="1:5" ht="18" x14ac:dyDescent="0.2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="229" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A229" t="s">
-        <v>299</v>
-      </c>
-      <c r="B229" t="s">
-        <v>300</v>
+        <v>70</v>
+      </c>
+      <c r="B229">
+        <v>472</v>
       </c>
       <c r="C229" t="s">
-        <v>148</v>
+        <v>163</v>
       </c>
       <c r="D229" t="s">
-        <v>253</v>
-      </c>
-      <c r="E229" s="4"/>
+        <v>4</v>
+      </c>
     </row>
     <row r="230" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A230" t="s">
-        <v>93</v>
-      </c>
-      <c r="B230" t="s">
-        <v>45</v>
+        <v>73</v>
+      </c>
+      <c r="B230">
+        <v>289</v>
       </c>
       <c r="C230" t="s">
-        <v>163</v>
+        <v>148</v>
       </c>
       <c r="D230" t="s">
         <v>4</v>
@@ -4600,10 +4811,10 @@
     </row>
     <row r="231" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A231" t="s">
-        <v>95</v>
-      </c>
-      <c r="B231" t="s">
-        <v>45</v>
+        <v>100</v>
+      </c>
+      <c r="B231">
+        <v>101</v>
       </c>
       <c r="C231" t="s">
         <v>163</v>
@@ -4614,13 +4825,13 @@
     </row>
     <row r="232" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A232" t="s">
-        <v>49</v>
+        <v>69</v>
       </c>
       <c r="B232">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C232" t="s">
-        <v>184</v>
+        <v>163</v>
       </c>
       <c r="D232" t="s">
         <v>4</v>
@@ -4628,13 +4839,13 @@
     </row>
     <row r="233" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A233" t="s">
-        <v>185</v>
+        <v>96</v>
       </c>
       <c r="B233">
-        <v>512</v>
+        <v>100</v>
       </c>
       <c r="C233" t="s">
-        <v>184</v>
+        <v>163</v>
       </c>
       <c r="D233" t="s">
         <v>4</v>
@@ -4642,13 +4853,13 @@
     </row>
     <row r="234" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A234" t="s">
-        <v>51</v>
+        <v>77</v>
       </c>
       <c r="B234">
         <v>0</v>
       </c>
       <c r="C234" t="s">
-        <v>184</v>
+        <v>148</v>
       </c>
       <c r="D234" t="s">
         <v>4</v>
@@ -4656,13 +4867,13 @@
     </row>
     <row r="235" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A235" t="s">
-        <v>170</v>
+        <v>75</v>
       </c>
       <c r="B235">
-        <v>100</v>
-      </c>
-      <c r="C235" s="3" t="s">
-        <v>163</v>
+        <v>4531</v>
+      </c>
+      <c r="C235" t="s">
+        <v>148</v>
       </c>
       <c r="D235" t="s">
         <v>4</v>
@@ -4670,13 +4881,13 @@
     </row>
     <row r="236" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A236" t="s">
-        <v>50</v>
+        <v>82</v>
       </c>
       <c r="B236" t="s">
         <v>45</v>
       </c>
       <c r="C236" t="s">
-        <v>184</v>
+        <v>148</v>
       </c>
       <c r="D236" t="s">
         <v>4</v>
@@ -4684,13 +4895,13 @@
     </row>
     <row r="237" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A237" t="s">
-        <v>52</v>
+        <v>67</v>
       </c>
       <c r="B237">
-        <v>104</v>
+        <v>203</v>
       </c>
       <c r="C237" t="s">
-        <v>184</v>
+        <v>186</v>
       </c>
       <c r="D237" t="s">
         <v>4</v>
@@ -4698,13 +4909,13 @@
     </row>
     <row r="238" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A238" t="s">
-        <v>135</v>
+        <v>66</v>
       </c>
       <c r="B238">
-        <v>471</v>
+        <v>203</v>
       </c>
       <c r="C238" t="s">
-        <v>108</v>
+        <v>186</v>
       </c>
       <c r="D238" t="s">
         <v>4</v>
@@ -4712,38 +4923,42 @@
     </row>
     <row r="239" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A239" t="s">
-        <v>126</v>
-      </c>
-      <c r="B239">
-        <v>105</v>
+        <v>316</v>
+      </c>
+      <c r="B239" t="s">
+        <v>300</v>
       </c>
       <c r="C239" t="s">
-        <v>108</v>
+        <v>148</v>
       </c>
       <c r="D239" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="240" spans="1:5" x14ac:dyDescent="0.2">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="240" spans="1:5" ht="18" x14ac:dyDescent="0.2">
       <c r="A240" t="s">
-        <v>124</v>
-      </c>
-      <c r="B240">
-        <v>105</v>
+        <v>292</v>
+      </c>
+      <c r="B240" t="s">
+        <v>293</v>
       </c>
       <c r="C240" t="s">
-        <v>108</v>
+        <v>148</v>
       </c>
       <c r="D240" t="s">
-        <v>4</v>
-      </c>
+        <v>253</v>
+      </c>
+      <c r="E240" s="3"/>
     </row>
     <row r="241" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A241" t="s">
-        <v>122</v>
+        <v>93</v>
+      </c>
+      <c r="B241" t="s">
+        <v>45</v>
       </c>
       <c r="C241" t="s">
-        <v>108</v>
+        <v>163</v>
       </c>
       <c r="D241" t="s">
         <v>4</v>
@@ -4751,13 +4966,13 @@
     </row>
     <row r="242" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A242" t="s">
-        <v>223</v>
-      </c>
-      <c r="B242">
-        <v>750</v>
+        <v>95</v>
+      </c>
+      <c r="B242" t="s">
+        <v>45</v>
       </c>
       <c r="C242" t="s">
-        <v>108</v>
+        <v>163</v>
       </c>
       <c r="D242" t="s">
         <v>4</v>
@@ -4765,13 +4980,13 @@
     </row>
     <row r="243" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A243" t="s">
-        <v>117</v>
+        <v>49</v>
       </c>
       <c r="B243">
-        <v>153</v>
+        <v>104</v>
       </c>
       <c r="C243" t="s">
-        <v>108</v>
+        <v>184</v>
       </c>
       <c r="D243" t="s">
         <v>4</v>
@@ -4779,13 +4994,13 @@
     </row>
     <row r="244" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A244" t="s">
-        <v>246</v>
+        <v>185</v>
       </c>
       <c r="B244">
-        <v>272</v>
+        <v>512</v>
       </c>
       <c r="C244" t="s">
-        <v>108</v>
+        <v>184</v>
       </c>
       <c r="D244" t="s">
         <v>4</v>
@@ -4793,13 +5008,13 @@
     </row>
     <row r="245" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A245" t="s">
-        <v>127</v>
+        <v>51</v>
       </c>
       <c r="B245">
-        <v>682</v>
+        <v>0</v>
       </c>
       <c r="C245" t="s">
-        <v>108</v>
+        <v>184</v>
       </c>
       <c r="D245" t="s">
         <v>4</v>
@@ -4807,13 +5022,13 @@
     </row>
     <row r="246" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A246" t="s">
-        <v>206</v>
+        <v>170</v>
       </c>
       <c r="B246">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C246" t="s">
-        <v>108</v>
+        <v>163</v>
       </c>
       <c r="D246" t="s">
         <v>4</v>
@@ -4821,13 +5036,13 @@
     </row>
     <row r="247" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A247" t="s">
-        <v>118</v>
-      </c>
-      <c r="B247">
-        <v>303</v>
+        <v>50</v>
+      </c>
+      <c r="B247" t="s">
+        <v>45</v>
       </c>
       <c r="C247" t="s">
-        <v>108</v>
+        <v>184</v>
       </c>
       <c r="D247" t="s">
         <v>4</v>
@@ -4835,13 +5050,13 @@
     </row>
     <row r="248" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A248" t="s">
-        <v>243</v>
+        <v>52</v>
       </c>
       <c r="B248">
-        <v>750</v>
+        <v>104</v>
       </c>
       <c r="C248" t="s">
-        <v>108</v>
+        <v>184</v>
       </c>
       <c r="D248" t="s">
         <v>4</v>
@@ -4849,10 +5064,10 @@
     </row>
     <row r="249" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A249" t="s">
-        <v>112</v>
+        <v>135</v>
       </c>
       <c r="B249">
-        <v>222</v>
+        <v>471</v>
       </c>
       <c r="C249" t="s">
         <v>108</v>
@@ -4863,10 +5078,10 @@
     </row>
     <row r="250" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A250" t="s">
-        <v>138</v>
+        <v>126</v>
       </c>
       <c r="B250">
-        <v>100</v>
+        <v>105</v>
       </c>
       <c r="C250" t="s">
         <v>108</v>
@@ -4877,10 +5092,10 @@
     </row>
     <row r="251" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A251" t="s">
-        <v>137</v>
+        <v>124</v>
       </c>
       <c r="B251">
-        <v>151</v>
+        <v>105</v>
       </c>
       <c r="C251" t="s">
         <v>108</v>
@@ -4891,10 +5106,7 @@
     </row>
     <row r="252" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A252" t="s">
-        <v>136</v>
-      </c>
-      <c r="B252">
-        <v>101</v>
+        <v>122</v>
       </c>
       <c r="C252" t="s">
         <v>108</v>
@@ -4905,7 +5117,7 @@
     </row>
     <row r="253" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A253" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="B253">
         <v>750</v>
@@ -4919,10 +5131,10 @@
     </row>
     <row r="254" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A254" t="s">
-        <v>228</v>
-      </c>
-      <c r="B254" t="s">
-        <v>229</v>
+        <v>117</v>
+      </c>
+      <c r="B254">
+        <v>153</v>
       </c>
       <c r="C254" t="s">
         <v>108</v>
@@ -4933,10 +5145,10 @@
     </row>
     <row r="255" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A255" t="s">
-        <v>232</v>
-      </c>
-      <c r="B255" t="s">
-        <v>229</v>
+        <v>246</v>
+      </c>
+      <c r="B255">
+        <v>272</v>
       </c>
       <c r="C255" t="s">
         <v>108</v>
@@ -4947,10 +5159,10 @@
     </row>
     <row r="256" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A256" t="s">
-        <v>224</v>
+        <v>127</v>
       </c>
       <c r="B256">
-        <v>750</v>
+        <v>682</v>
       </c>
       <c r="C256" t="s">
         <v>108</v>
@@ -4961,10 +5173,10 @@
     </row>
     <row r="257" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A257" t="s">
-        <v>250</v>
+        <v>206</v>
       </c>
       <c r="B257">
-        <v>203</v>
+        <v>102</v>
       </c>
       <c r="C257" t="s">
         <v>108</v>
@@ -4975,10 +5187,10 @@
     </row>
     <row r="258" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A258" t="s">
-        <v>249</v>
+        <v>118</v>
       </c>
       <c r="B258">
-        <v>752</v>
+        <v>303</v>
       </c>
       <c r="C258" t="s">
         <v>108</v>
@@ -4989,7 +5201,7 @@
     </row>
     <row r="259" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A259" t="s">
-        <v>225</v>
+        <v>243</v>
       </c>
       <c r="B259">
         <v>750</v>
@@ -5003,10 +5215,10 @@
     </row>
     <row r="260" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A260" t="s">
-        <v>248</v>
+        <v>112</v>
       </c>
       <c r="B260">
-        <v>333</v>
+        <v>222</v>
       </c>
       <c r="C260" t="s">
         <v>108</v>
@@ -5017,10 +5229,10 @@
     </row>
     <row r="261" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A261" t="s">
-        <v>116</v>
+        <v>138</v>
       </c>
       <c r="B261">
-        <v>393</v>
+        <v>100</v>
       </c>
       <c r="C261" t="s">
         <v>108</v>
@@ -5031,10 +5243,10 @@
     </row>
     <row r="262" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A262" t="s">
-        <v>119</v>
+        <v>137</v>
       </c>
       <c r="B262">
-        <v>123</v>
+        <v>151</v>
       </c>
       <c r="C262" t="s">
         <v>108</v>
@@ -5045,10 +5257,10 @@
     </row>
     <row r="263" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A263" t="s">
-        <v>242</v>
+        <v>136</v>
       </c>
       <c r="B263">
-        <v>331</v>
+        <v>101</v>
       </c>
       <c r="C263" t="s">
         <v>108</v>
@@ -5059,10 +5271,10 @@
     </row>
     <row r="264" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A264" t="s">
-        <v>241</v>
+        <v>226</v>
       </c>
       <c r="B264">
-        <v>331</v>
+        <v>750</v>
       </c>
       <c r="C264" t="s">
         <v>108</v>
@@ -5073,21 +5285,175 @@
     </row>
     <row r="265" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A265" t="s">
+        <v>228</v>
+      </c>
+      <c r="B265" t="s">
+        <v>229</v>
+      </c>
+      <c r="C265" t="s">
+        <v>108</v>
+      </c>
+      <c r="D265" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="266" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A266" t="s">
+        <v>232</v>
+      </c>
+      <c r="B266" t="s">
+        <v>229</v>
+      </c>
+      <c r="C266" t="s">
+        <v>108</v>
+      </c>
+      <c r="D266" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="267" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A267" t="s">
+        <v>224</v>
+      </c>
+      <c r="B267">
+        <v>750</v>
+      </c>
+      <c r="C267" t="s">
+        <v>108</v>
+      </c>
+      <c r="D267" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="268" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A268" t="s">
+        <v>250</v>
+      </c>
+      <c r="B268">
+        <v>203</v>
+      </c>
+      <c r="C268" t="s">
+        <v>108</v>
+      </c>
+      <c r="D268" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="269" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A269" t="s">
+        <v>249</v>
+      </c>
+      <c r="B269">
+        <v>752</v>
+      </c>
+      <c r="C269" t="s">
+        <v>108</v>
+      </c>
+      <c r="D269" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="270" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A270" t="s">
+        <v>225</v>
+      </c>
+      <c r="B270">
+        <v>750</v>
+      </c>
+      <c r="C270" t="s">
+        <v>108</v>
+      </c>
+      <c r="D270" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="271" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A271" t="s">
+        <v>248</v>
+      </c>
+      <c r="B271">
+        <v>333</v>
+      </c>
+      <c r="C271" t="s">
+        <v>108</v>
+      </c>
+      <c r="D271" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="272" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A272" t="s">
+        <v>116</v>
+      </c>
+      <c r="B272">
+        <v>393</v>
+      </c>
+      <c r="C272" t="s">
+        <v>108</v>
+      </c>
+      <c r="D272" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="273" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A273" t="s">
+        <v>119</v>
+      </c>
+      <c r="B273">
+        <v>123</v>
+      </c>
+      <c r="C273" t="s">
+        <v>108</v>
+      </c>
+      <c r="D273" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="274" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A274" t="s">
+        <v>242</v>
+      </c>
+      <c r="B274">
+        <v>331</v>
+      </c>
+      <c r="C274" t="s">
+        <v>108</v>
+      </c>
+      <c r="D274" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="275" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A275" t="s">
+        <v>241</v>
+      </c>
+      <c r="B275">
+        <v>331</v>
+      </c>
+      <c r="C275" t="s">
+        <v>108</v>
+      </c>
+      <c r="D275" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="276" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A276" t="s">
         <v>240</v>
       </c>
-      <c r="B265">
+      <c r="B276">
         <v>331</v>
       </c>
-      <c r="C265" t="s">
-        <v>108</v>
-      </c>
-      <c r="D265" t="s">
+      <c r="C276" t="s">
+        <v>108</v>
+      </c>
+      <c r="D276" t="s">
         <v>4</v>
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="3" type="noConversion"/>
-  <conditionalFormatting sqref="A1:A227 B228 A229:A1075">
+  <phoneticPr fontId="4" type="noConversion"/>
+  <conditionalFormatting sqref="A277:A1084 A1:A186 B187 A188:A222">
     <cfRule type="duplicateValues" dxfId="0" priority="43" stopIfTrue="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>